<commit_message>
add one-way ANOVA test
</commit_message>
<xml_diff>
--- a/output_data/loose_bound_water_best_subset_poly_regression_C_format.xlsx
+++ b/output_data/loose_bound_water_best_subset_poly_regression_C_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titus\Documents\Classes\NEUP\TGA_mass_loss\output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DF131E87-7FC0-4E2C-BCA1-8120D3A0E182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9989EF71-43A5-4D81-8A12-F87F8048B1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loose_bound_water_best_subset_p" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Index(['Concentration(mM)', 'L/S^2'], dtype='object')</t>
   </si>
   <si>
-    <t>Index(['L/S', 'Concentration(mM)^2'], dtype='object')</t>
-  </si>
-  <si>
     <t>Index(['L/S', 'Concentration(mM) L/S'], dtype='object')</t>
   </si>
   <si>
@@ -244,12 +241,15 @@
     <t>Index(['1', 'Concentration(mM)', 'L/S', 'Concentration(mM)^2',
        'Concentration(mM) L/S', 'L/S^2'],
       dtype='object')</t>
+  </si>
+  <si>
+    <t>Index([], dtype='object')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -794,67 +794,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="281">
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -1057,56 +997,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -1182,2406 +1072,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF66FF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3914,7 +1404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -4344,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
@@ -4370,7 +1860,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -4396,7 +1886,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2">
         <v>2</v>
@@ -4422,7 +1912,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -4448,7 +1938,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2">
         <v>2</v>
@@ -4474,7 +1964,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2">
         <v>2</v>
@@ -4500,7 +1990,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -4526,7 +2016,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -4552,7 +2042,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -4578,7 +2068,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -4604,7 +2094,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -4630,7 +2120,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -4656,7 +2146,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -4682,7 +2172,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -4708,7 +2198,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -4734,7 +2224,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -4760,7 +2250,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -4786,7 +2276,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -4812,7 +2302,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -4838,7 +2328,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -4864,7 +2354,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -4890,7 +2380,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -4916,7 +2406,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -4942,7 +2432,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -4968,7 +2458,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -4994,7 +2484,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42">
         <v>3</v>
@@ -5020,7 +2510,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="2">
         <v>4</v>
@@ -5046,7 +2536,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="2">
         <v>4</v>
@@ -5072,7 +2562,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45" s="2">
         <v>4</v>
@@ -5098,7 +2588,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" s="2">
         <v>4</v>
@@ -5124,7 +2614,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" s="2">
         <v>4</v>
@@ -5150,7 +2640,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48" s="2">
         <v>4</v>
@@ -5176,7 +2666,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" s="2">
         <v>4</v>
@@ -5202,7 +2692,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" s="2">
         <v>4</v>
@@ -5228,7 +2718,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" s="2">
         <v>4</v>
@@ -5254,7 +2744,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52" s="2">
         <v>4</v>
@@ -5280,7 +2770,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="2">
         <v>4</v>
@@ -5306,7 +2796,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" s="2">
         <v>4</v>
@@ -5332,7 +2822,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" s="2">
         <v>4</v>
@@ -5358,7 +2848,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="2">
         <v>4</v>
@@ -5384,7 +2874,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
@@ -5410,7 +2900,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -5436,7 +2926,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -5462,7 +2952,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -5488,7 +2978,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -5514,7 +3004,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -5540,7 +3030,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -5566,7 +3056,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64">
         <v>6</v>
@@ -5604,7 +3094,7 @@
     <row r="79" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="H2:H7">
-    <cfRule type="top10" dxfId="90" priority="108" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="108" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
@@ -5617,7 +3107,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="top10" dxfId="89" priority="106" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="106" rank="1"/>
     <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
@@ -5630,7 +3120,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H22">
-    <cfRule type="top10" dxfId="87" priority="93" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="27" priority="93" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
@@ -5643,7 +3133,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F22">
-    <cfRule type="top10" dxfId="86" priority="91" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="91" rank="1"/>
     <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min"/>
@@ -5656,7 +3146,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:H42">
-    <cfRule type="top10" dxfId="84" priority="78" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="78" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
@@ -5669,7 +3159,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F42">
-    <cfRule type="top10" dxfId="83" priority="76" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="76" rank="1"/>
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
@@ -5682,7 +3172,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H57">
-    <cfRule type="top10" dxfId="81" priority="63" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="63" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -5695,7 +3185,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:F57">
-    <cfRule type="top10" dxfId="80" priority="61" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="61" rank="1"/>
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -5708,10 +3198,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H64">
-    <cfRule type="top10" dxfId="79" priority="60" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="60" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58:H64">
-    <cfRule type="top10" dxfId="77" priority="48" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="48" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -5724,7 +3214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58:F64">
-    <cfRule type="top10" dxfId="76" priority="46" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="46" rank="1"/>
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -5737,7 +3227,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7">
-    <cfRule type="top10" dxfId="74" priority="33" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="33" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -5750,7 +3240,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G22">
-    <cfRule type="top10" dxfId="73" priority="31" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="31" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -5763,7 +3253,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:G42">
-    <cfRule type="top10" dxfId="72" priority="29" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="29" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -5776,7 +3266,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G57">
-    <cfRule type="top10" dxfId="71" priority="27" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="27" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -5789,10 +3279,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G64">
-    <cfRule type="top10" dxfId="70" priority="26" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="26" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58:G64">
-    <cfRule type="top10" dxfId="69" priority="24" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="24" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -5805,7 +3295,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D7">
-    <cfRule type="top10" dxfId="68" priority="22" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="22" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -5818,7 +3308,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D22">
-    <cfRule type="top10" dxfId="67" priority="20" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="20" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -5831,7 +3321,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D42">
-    <cfRule type="top10" dxfId="66" priority="18" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="18" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -5844,7 +3334,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D57">
-    <cfRule type="top10" dxfId="65" priority="16" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="16" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -5857,10 +3347,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D64">
-    <cfRule type="top10" dxfId="64" priority="15" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="15" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58:D64">
-    <cfRule type="top10" dxfId="63" priority="13" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="13" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -5873,7 +3363,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F64">
-    <cfRule type="top10" dxfId="12" priority="12" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="12" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E7">
     <cfRule type="top10" dxfId="5" priority="10" rank="1"/>

</xml_diff>